<commit_message>
improve structure, sensor recv by FSM
</commit_message>
<xml_diff>
--- a/Doc/DataFormat.xlsx
+++ b/Doc/DataFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git_repository\OurEDA\ROV_SensorBoard\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3466109D-3651-4163-86DA-A429E17ABEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFB7D8A-C940-4409-9416-A162A6F9BA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>起始位</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,7 +135,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>舱温舱湿为乘10后结果</t>
+    <t>所有数据位均按uint16_t解读</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位摄氏度℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>压力单位为Pa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水深为乘1000后结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位米m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>舱温舱湿为乘1000后结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水温为乘100后结果</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -194,10 +218,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -484,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -496,35 +519,35 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="3"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -557,16 +580,16 @@
       <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -601,28 +624,48 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H5" s="3" t="s">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="O5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="L7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
improve structure, add sonar-GP30 driver supporting
</commit_message>
<xml_diff>
--- a/Doc/DataFormat.xlsx
+++ b/Doc/DataFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git_repository\OurEDA\ROV_SensorBoard\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFB7D8A-C940-4409-9416-A162A6F9BA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F0E3D0-AD6F-45A2-87B7-308A65FA4C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
   <si>
     <t>起始位</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -160,6 +160,30 @@
   </si>
   <si>
     <t>水温为乘100后结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有数据位均按uint解读</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dist_HL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dist_HH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dist_LH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dist_LL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -507,15 +531,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +573,7 @@
       </c>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -599,7 +623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -623,7 +647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -639,7 +663,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H6" s="3" t="s">
         <v>19</v>
       </c>
@@ -649,7 +673,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H7" s="2" t="s">
         <v>18</v>
       </c>
@@ -662,13 +686,197 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L8" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T15" s="2"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="L19" t="s">
+        <v>33</v>
+      </c>
+      <c r="O19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="L20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="L21" t="s">
+        <v>30</v>
+      </c>
+      <c r="O21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="19">
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:G1"/>

</xml_diff>